<commit_message>
update pinout Excel file
</commit_message>
<xml_diff>
--- a/_Version/MAXV2380_Pinout.xlsx
+++ b/_Version/MAXV2380_Pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onarce\OneDrive - EFS\Bureau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mes documents\P-CAD_PROJECTS\_PROJETS_ON\PROJECTS\Git\_Logiciels_KICAD\AA2380_MAXV\_Version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{A815C3A5-72F6-4E35-89D6-700312AFD447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76F01E1-6D91-4DBA-943A-6426399C6A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AA2380_MAXV" sheetId="2" r:id="rId1"/>
@@ -36,15 +36,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Requête - AA2380_MAXV" description="Connexion à la requête « AA2380_MAXV » dans le classeur." type="5" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Requête - AA2380_MAXV" description="Connexion à la requête « AA2380_MAXV » dans le classeur." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=AA2380_MAXV;Extended Properties=&quot;&quot;" command="SELECT * FROM [AA2380_MAXV]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="226">
   <si>
     <t/>
   </si>
@@ -677,13 +677,58 @@
   </si>
   <si>
     <t>5M570ZT100C5N</t>
+  </si>
+  <si>
+    <t>Pin n°</t>
+  </si>
+  <si>
+    <t>J12-AA2380</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>+3V3</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>DFS0</t>
+  </si>
+  <si>
+    <t>DFS1</t>
+  </si>
+  <si>
+    <t>DFS2</t>
+  </si>
+  <si>
+    <t>nRESET</t>
+  </si>
+  <si>
+    <t>I2S_BCK</t>
+  </si>
+  <si>
+    <t>I2S_LRCK</t>
+  </si>
+  <si>
+    <t>I2S_DATA</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Src/Dest</t>
+  </si>
+  <si>
+    <t>USB-I2S board</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -713,8 +758,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -805,8 +866,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -943,11 +1010,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -967,6 +1134,181 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -976,182 +1318,62 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1199,41 +1421,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1346,13 +1533,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1366,6 +1546,48 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1382,7 +1604,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DonnéesExternes_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DonnéesExternes_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="15" unboundColumnsRight="3">
     <queryTableFields count="8">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
@@ -1407,22 +1629,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="AA2380_MAXV" displayName="AA2380_MAXV" ref="B4:I77" tableType="queryTable" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
-  <autoFilter ref="B4:I77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="AA2380_MAXV" displayName="AA2380_MAXV" ref="B4:I77" tableType="queryTable" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="B4:I77" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:H77">
     <sortCondition ref="C4:C77"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" uniqueName="1" name="Signal Name" queryTableFieldId="1" dataDxfId="9"/>
-    <tableColumn id="2" uniqueName="2" name="Direction" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" uniqueName="3" name="Pin Number" queryTableFieldId="3" dataDxfId="7"/>
-    <tableColumn id="4" uniqueName="4" name="I/O Bank" queryTableFieldId="4" dataDxfId="6"/>
-    <tableColumn id="10" uniqueName="10" name="Pull-up" queryTableFieldId="10" dataDxfId="5"/>
-    <tableColumn id="13" uniqueName="13" name="Colonne1" queryTableFieldId="13" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Signal Name" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Direction" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Pin Number" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="I/O Bank" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="10" name="Pull-up" queryTableFieldId="10" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" uniqueName="13" name="Colonne1" queryTableFieldId="13" dataDxfId="2">
       <calculatedColumnFormula>MID(D5,5,LEN(C5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" uniqueName="12" name="Signal Name2" queryTableFieldId="12" dataDxfId="1"/>
-    <tableColumn id="14" uniqueName="14" name="Fonctionnal description" queryTableFieldId="14" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" uniqueName="12" name="Signal Name2" queryTableFieldId="12" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" uniqueName="14" name="Fonctionnal description" queryTableFieldId="14" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1724,11 +1946,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1756,19 +1978,19 @@
         <v>210</v>
       </c>
       <c r="F1" s="69"/>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="65" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="66" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="68"/>
       <c r="H3" s="5" t="s">
         <v>158</v>
       </c>
@@ -1803,2045 +2025,2045 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="13" t="str">
-        <f>MID(D5,5,LEN(C5))</f>
+      <c r="G5" s="10" t="str">
+        <f t="shared" ref="G5:G36" si="0">MID(D5,5,LEN(C5))</f>
         <v>35</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="I5" s="66"/>
+      <c r="I5" s="63"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="13" t="str">
-        <f>MID(D6,5,LEN(C6))</f>
+      <c r="F6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="I6" s="66"/>
+      <c r="I6" s="63"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="13" t="str">
-        <f>MID(D7,5,LEN(C7))</f>
+      <c r="F7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="I7" s="66"/>
+      <c r="I7" s="63"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="13" t="str">
-        <f>MID(D8,5,LEN(C8))</f>
+      <c r="G8" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="I8" s="66"/>
+      <c r="I8" s="63"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="13" t="str">
-        <f>MID(D9,5,LEN(C9))</f>
+      <c r="G9" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="I9" s="66"/>
+      <c r="I9" s="63"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="17" t="str">
-        <f>MID(D10,5,LEN(C10))</f>
+      <c r="G10" s="14" t="str">
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="I10" s="66"/>
+      <c r="I10" s="63"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="17" t="str">
-        <f>MID(D11,5,LEN(C11))</f>
+      <c r="G11" s="14" t="str">
+        <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="I11" s="66"/>
+      <c r="I11" s="63"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="17" t="str">
-        <f>MID(D12,5,LEN(C12))</f>
+      <c r="G12" s="14" t="str">
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="I12" s="66"/>
+      <c r="I12" s="63"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="21" t="str">
-        <f>MID(D13,5,LEN(C13))</f>
+      <c r="G13" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="66"/>
+      <c r="I13" s="63"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="21" t="str">
-        <f>MID(D14,5,LEN(C14))</f>
+      <c r="G14" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="66"/>
+      <c r="I14" s="63"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="21" t="str">
-        <f>MID(D15,5,LEN(C15))</f>
+      <c r="G15" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="66"/>
+      <c r="I15" s="63"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="21" t="str">
-        <f>MID(D16,5,LEN(C16))</f>
+      <c r="G16" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="66"/>
+      <c r="I16" s="63"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="21" t="str">
-        <f>MID(D17,5,LEN(C17))</f>
+      <c r="G17" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="I17" s="66"/>
+      <c r="I17" s="63"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="21" t="str">
-        <f>MID(D18,5,LEN(C18))</f>
+      <c r="G18" s="18" t="str">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="66"/>
+      <c r="I18" s="63"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="25" t="str">
-        <f>MID(D19,5,LEN(C19))</f>
+      <c r="G19" s="22" t="str">
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="I19" s="66"/>
+      <c r="I19" s="63"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="25" t="str">
-        <f>MID(D20,5,LEN(C20))</f>
+      <c r="G20" s="22" t="str">
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="I20" s="66"/>
+      <c r="I20" s="63"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="25" t="str">
-        <f>MID(D21,5,LEN(C21))</f>
+      <c r="G21" s="22" t="str">
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="I21" s="66"/>
+      <c r="I21" s="63"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="25" t="str">
-        <f>MID(D22,5,LEN(C22))</f>
+      <c r="G22" s="22" t="str">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="I22" s="66"/>
+      <c r="I22" s="63"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" s="29" t="str">
-        <f>MID(D23,5,LEN(C23))</f>
+      <c r="F23" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="H23" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="I23" s="66"/>
+      <c r="I23" s="63"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="G24" s="29" t="str">
-        <f>MID(D24,5,LEN(C24))</f>
+      <c r="F24" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="66"/>
+      <c r="I24" s="63"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" s="29" t="str">
-        <f>MID(D25,5,LEN(C25))</f>
+      <c r="F25" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="66"/>
+      <c r="I25" s="63"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" s="33" t="str">
-        <f>MID(D26,5,LEN(C26))</f>
+      <c r="F26" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="I26" s="66"/>
+      <c r="I26" s="63"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G27" s="33" t="str">
-        <f>MID(D27,5,LEN(C27))</f>
+      <c r="F27" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="H27" s="31" t="s">
+      <c r="H27" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="I27" s="66"/>
+      <c r="I27" s="63"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="33" t="str">
-        <f>MID(D28,5,LEN(C28))</f>
+      <c r="F28" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="H28" s="31" t="s">
+      <c r="H28" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="I28" s="66"/>
+      <c r="I28" s="63"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" s="33" t="str">
-        <f>MID(D29,5,LEN(C29))</f>
+      <c r="F29" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="H29" s="31" t="s">
+      <c r="H29" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="I29" s="66"/>
+      <c r="I29" s="63"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="11" t="s">
+      <c r="C30" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G30" s="13" t="str">
-        <f>MID(D30,5,LEN(C30))</f>
+      <c r="F30" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="I30" s="66"/>
+      <c r="I30" s="63"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="11" t="s">
+      <c r="C31" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G31" s="13" t="str">
-        <f>MID(D31,5,LEN(C31))</f>
+      <c r="F31" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="I31" s="66"/>
+      <c r="I31" s="63"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="11" t="s">
+      <c r="C32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G32" s="13" t="str">
-        <f>MID(D32,5,LEN(C32))</f>
+      <c r="F32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="I32" s="66"/>
+      <c r="I32" s="63"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="11" t="s">
+      <c r="C33" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G33" s="13" t="str">
-        <f>MID(D33,5,LEN(C33))</f>
+      <c r="F33" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H33" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I33" s="66"/>
+      <c r="I33" s="63"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="11" t="s">
+      <c r="C34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G34" s="13" t="str">
-        <f>MID(D34,5,LEN(C34))</f>
+      <c r="F34" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="H34" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="I34" s="66"/>
+      <c r="I34" s="63"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="11" t="s">
+      <c r="C35" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" s="13" t="str">
-        <f>MID(D35,5,LEN(C35))</f>
+      <c r="F35" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10" t="str">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H35" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="I35" s="66"/>
+      <c r="I35" s="63"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>32</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="C36" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="35" t="s">
+      <c r="C36" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="E36" s="35" t="s">
+      <c r="E36" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="G36" s="37" t="str">
-        <f>MID(D36,5,LEN(C36))</f>
+      <c r="F36" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="34" t="str">
+        <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="H36" s="35" t="s">
+      <c r="H36" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="I36" s="66"/>
+      <c r="I36" s="63"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>33</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="39" t="s">
+      <c r="C37" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="E37" s="39" t="s">
+      <c r="E37" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G37" s="41" t="str">
-        <f>MID(D37,5,LEN(C37))</f>
+      <c r="F37" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="38" t="str">
+        <f t="shared" ref="G37:G68" si="1">MID(D37,5,LEN(C37))</f>
         <v>48</v>
       </c>
-      <c r="H37" s="39" t="s">
+      <c r="H37" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="I37" s="66"/>
+      <c r="I37" s="63"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>34</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="39" t="s">
+      <c r="C38" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="E38" s="39" t="s">
+      <c r="E38" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F38" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G38" s="41" t="str">
-        <f>MID(D38,5,LEN(C38))</f>
+      <c r="F38" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="38" t="str">
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="H38" s="39" t="s">
+      <c r="H38" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="I38" s="66"/>
+      <c r="I38" s="63"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>35</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="C39" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="43" t="s">
+      <c r="C39" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="E39" s="43" t="s">
+      <c r="E39" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="G39" s="45" t="str">
-        <f>MID(D39,5,LEN(C39))</f>
+      <c r="F39" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="42" t="str">
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="H39" s="43" t="s">
+      <c r="H39" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="I39" s="66"/>
+      <c r="I39" s="63"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>36</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="43" t="s">
+      <c r="C40" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="E40" s="43" t="s">
+      <c r="E40" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="G40" s="45" t="str">
-        <f>MID(D40,5,LEN(C40))</f>
+      <c r="F40" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="42" t="str">
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="H40" s="43" t="s">
+      <c r="H40" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="I40" s="66"/>
+      <c r="I40" s="63"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>37</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="C41" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="47" t="s">
+      <c r="C41" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="47" t="s">
+      <c r="E41" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="G41" s="49" t="str">
-        <f>MID(D41,5,LEN(C41))</f>
+      <c r="F41" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="46" t="str">
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="H41" s="47" t="s">
+      <c r="H41" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="I41" s="66"/>
+      <c r="I41" s="63"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>38</v>
       </c>
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="47" t="s">
+      <c r="C42" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="E42" s="47" t="s">
+      <c r="E42" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F42" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="G42" s="49" t="str">
-        <f>MID(D42,5,LEN(C42))</f>
+      <c r="F42" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="46" t="str">
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="H42" s="47" t="s">
+      <c r="H42" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="I42" s="66"/>
+      <c r="I42" s="63"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>39</v>
       </c>
-      <c r="B43" s="46" t="s">
+      <c r="B43" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="C43" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="47" t="s">
+      <c r="C43" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="E43" s="47" t="s">
+      <c r="E43" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F43" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="G43" s="49" t="str">
-        <f>MID(D43,5,LEN(C43))</f>
+      <c r="F43" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" s="46" t="str">
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="H43" s="47" t="s">
+      <c r="H43" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="I43" s="66"/>
+      <c r="I43" s="63"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>40</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="51" t="s">
+      <c r="C44" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="51" t="s">
+      <c r="E44" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F44" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G44" s="53" t="str">
-        <f>MID(D44,5,LEN(C44))</f>
+      <c r="F44" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H44" s="51" t="s">
+      <c r="H44" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="I44" s="66"/>
+      <c r="I44" s="63"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="51" t="s">
+      <c r="C45" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="51" t="s">
+      <c r="E45" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F45" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G45" s="53" t="str">
-        <f>MID(D45,5,LEN(C45))</f>
+      <c r="F45" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H45" s="51" t="s">
+      <c r="H45" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="I45" s="66"/>
+      <c r="I45" s="63"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="51" t="s">
+      <c r="C46" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="E46" s="51" t="s">
+      <c r="E46" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F46" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G46" s="53" t="str">
-        <f>MID(D46,5,LEN(C46))</f>
+      <c r="F46" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="H46" s="51" t="s">
+      <c r="H46" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="I46" s="66"/>
+      <c r="I46" s="63"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43</v>
       </c>
-      <c r="B47" s="50" t="s">
+      <c r="B47" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="51" t="s">
+      <c r="C47" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E47" s="51" t="s">
+      <c r="E47" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F47" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G47" s="53" t="str">
-        <f>MID(D47,5,LEN(C47))</f>
+      <c r="F47" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G47" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="H47" s="51" t="s">
+      <c r="H47" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="I47" s="66"/>
+      <c r="I47" s="63"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="51" t="s">
+      <c r="C48" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="E48" s="51" t="s">
+      <c r="E48" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F48" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G48" s="53" t="str">
-        <f>MID(D48,5,LEN(C48))</f>
+      <c r="F48" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="H48" s="51" t="s">
+      <c r="H48" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="I48" s="66"/>
+      <c r="I48" s="63"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="51" t="s">
+      <c r="C49" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="51" t="s">
+      <c r="E49" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F49" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G49" s="53" t="str">
-        <f>MID(D49,5,LEN(C49))</f>
+      <c r="F49" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G49" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="H49" s="51" t="s">
+      <c r="H49" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="I49" s="66"/>
+      <c r="I49" s="63"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>46</v>
       </c>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="51" t="s">
+      <c r="C50" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="E50" s="51" t="s">
+      <c r="E50" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F50" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G50" s="53" t="str">
-        <f>MID(D50,5,LEN(C50))</f>
+      <c r="F50" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="H50" s="51" t="s">
+      <c r="H50" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I50" s="66"/>
+      <c r="I50" s="63"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>47</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="51" t="s">
+      <c r="C51" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="E51" s="51" t="s">
+      <c r="E51" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F51" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G51" s="53" t="str">
-        <f>MID(D51,5,LEN(C51))</f>
+      <c r="F51" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="H51" s="51" t="s">
+      <c r="H51" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="I51" s="66"/>
+      <c r="I51" s="63"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>48</v>
       </c>
-      <c r="B52" s="50" t="s">
+      <c r="B52" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="51" t="s">
+      <c r="C52" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="E52" s="51" t="s">
+      <c r="E52" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F52" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G52" s="53" t="str">
-        <f>MID(D52,5,LEN(C52))</f>
+      <c r="F52" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G52" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H52" s="51" t="s">
+      <c r="H52" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="I52" s="66"/>
+      <c r="I52" s="63"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>49</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="51" t="s">
+      <c r="C53" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="E53" s="51" t="s">
+      <c r="E53" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F53" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G53" s="53" t="str">
-        <f>MID(D53,5,LEN(C53))</f>
+      <c r="F53" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G53" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H53" s="51" t="s">
+      <c r="H53" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="I53" s="66"/>
+      <c r="I53" s="63"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>50</v>
       </c>
-      <c r="B54" s="50" t="s">
+      <c r="B54" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="51" t="s">
+      <c r="C54" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="51" t="s">
+      <c r="E54" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F54" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G54" s="53" t="str">
-        <f>MID(D54,5,LEN(C54))</f>
+      <c r="F54" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G54" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H54" s="51" t="s">
+      <c r="H54" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="I54" s="66"/>
+      <c r="I54" s="63"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>51</v>
       </c>
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="51" t="s">
+      <c r="C55" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="E55" s="51" t="s">
+      <c r="E55" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F55" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G55" s="53" t="str">
-        <f>MID(D55,5,LEN(C55))</f>
+      <c r="F55" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G55" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="H55" s="51" t="s">
+      <c r="H55" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="I55" s="66"/>
+      <c r="I55" s="63"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>52</v>
       </c>
-      <c r="B56" s="54" t="s">
+      <c r="B56" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="55" t="s">
+      <c r="C56" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E56" s="55" t="s">
+      <c r="E56" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G56" s="57" t="str">
-        <f>MID(D56,5,LEN(C56))</f>
+      <c r="F56" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G56" s="54" t="str">
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="H56" s="55" t="s">
+      <c r="H56" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="I56" s="66"/>
+      <c r="I56" s="63"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>53</v>
       </c>
-      <c r="B57" s="54" t="s">
+      <c r="B57" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="55" t="s">
+      <c r="C57" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="E57" s="55" t="s">
+      <c r="E57" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F57" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G57" s="57" t="str">
-        <f>MID(D57,5,LEN(C57))</f>
+      <c r="F57" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G57" s="54" t="str">
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="H57" s="55" t="s">
+      <c r="H57" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="I57" s="66"/>
+      <c r="I57" s="63"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>54</v>
       </c>
-      <c r="B58" s="54" t="s">
+      <c r="B58" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="55" t="s">
+      <c r="C58" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="E58" s="55" t="s">
+      <c r="E58" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F58" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G58" s="57" t="str">
-        <f>MID(D58,5,LEN(C58))</f>
+      <c r="F58" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G58" s="54" t="str">
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="H58" s="55" t="s">
+      <c r="H58" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="I58" s="66"/>
+      <c r="I58" s="63"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>55</v>
       </c>
-      <c r="B59" s="54" t="s">
+      <c r="B59" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="55" t="s">
+      <c r="C59" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="E59" s="55" t="s">
+      <c r="E59" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F59" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G59" s="57" t="str">
-        <f>MID(D59,5,LEN(C59))</f>
+      <c r="F59" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G59" s="54" t="str">
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="H59" s="55" t="s">
+      <c r="H59" s="52" t="s">
         <v>198</v>
       </c>
-      <c r="I59" s="66"/>
+      <c r="I59" s="63"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>56</v>
       </c>
-      <c r="B60" s="54" t="s">
+      <c r="B60" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="C60" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="55" t="s">
+      <c r="C60" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="E60" s="55" t="s">
+      <c r="E60" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G60" s="57" t="str">
-        <f>MID(D60,5,LEN(C60))</f>
+      <c r="F60" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G60" s="54" t="str">
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="H60" s="55" t="s">
+      <c r="H60" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="I60" s="66"/>
+      <c r="I60" s="63"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>57</v>
       </c>
-      <c r="B61" s="58" t="s">
+      <c r="B61" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="59" t="s">
+      <c r="C61" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="E61" s="59" t="s">
+      <c r="E61" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="F61" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="G61" s="61" t="str">
-        <f>MID(D61,5,LEN(C61))</f>
+      <c r="F61" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="G61" s="58" t="str">
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="H61" s="59" t="s">
+      <c r="H61" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="I61" s="66"/>
+      <c r="I61" s="63"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>58</v>
       </c>
-      <c r="B62" s="58" t="s">
+      <c r="B62" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="C62" s="59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="59" t="s">
+      <c r="C62" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="E62" s="59" t="s">
+      <c r="E62" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="F62" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="G62" s="61" t="str">
-        <f>MID(D62,5,LEN(C62))</f>
+      <c r="F62" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="G62" s="58" t="str">
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="H62" s="59" t="s">
+      <c r="H62" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="I62" s="66"/>
+      <c r="I62" s="63"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>59</v>
       </c>
-      <c r="B63" s="58" t="s">
+      <c r="B63" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C63" s="59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="59" t="s">
+      <c r="C63" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="E63" s="59" t="s">
+      <c r="E63" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="F63" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="G63" s="61" t="str">
-        <f>MID(D63,5,LEN(C63))</f>
+      <c r="F63" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="G63" s="58" t="str">
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="H63" s="59" t="s">
+      <c r="H63" s="56" t="s">
         <v>182</v>
       </c>
-      <c r="I63" s="66"/>
+      <c r="I63" s="63"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>60</v>
       </c>
-      <c r="B64" s="54" t="s">
+      <c r="B64" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="55" t="s">
+      <c r="C64" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="E64" s="55" t="s">
+      <c r="E64" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F64" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G64" s="57" t="str">
-        <f>MID(D64,5,LEN(C64))</f>
+      <c r="F64" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" s="54" t="str">
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="H64" s="55" t="s">
+      <c r="H64" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="I64" s="66"/>
+      <c r="I64" s="63"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>61</v>
       </c>
-      <c r="B65" s="58" t="s">
+      <c r="B65" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="59" t="s">
+      <c r="C65" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="E65" s="59" t="s">
+      <c r="E65" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="F65" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="G65" s="61" t="str">
-        <f>MID(D65,5,LEN(C65))</f>
+      <c r="F65" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="G65" s="58" t="str">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="H65" s="59" t="s">
+      <c r="H65" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="I65" s="66"/>
+      <c r="I65" s="63"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>62</v>
       </c>
-      <c r="B66" s="58" t="s">
+      <c r="B66" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="C66" s="59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="59" t="s">
+      <c r="C66" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="E66" s="59" t="s">
+      <c r="E66" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="F66" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="G66" s="61" t="str">
-        <f>MID(D66,5,LEN(C66))</f>
+      <c r="F66" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="G66" s="58" t="str">
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="H66" s="59" t="s">
+      <c r="H66" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="I66" s="66"/>
+      <c r="I66" s="63"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>63</v>
       </c>
-      <c r="B67" s="58" t="s">
+      <c r="B67" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="C67" s="59" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="59" t="s">
+      <c r="C67" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="E67" s="59" t="s">
+      <c r="E67" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="F67" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="G67" s="61" t="str">
-        <f>MID(D67,5,LEN(C67))</f>
+      <c r="F67" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="G67" s="58" t="str">
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="H67" s="59" t="s">
+      <c r="H67" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="I67" s="66"/>
+      <c r="I67" s="63"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>64</v>
       </c>
-      <c r="B68" s="54" t="s">
+      <c r="B68" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="C68" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="55" t="s">
+      <c r="C68" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="E68" s="55" t="s">
+      <c r="E68" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F68" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G68" s="57" t="str">
-        <f>MID(D68,5,LEN(C68))</f>
+      <c r="F68" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G68" s="54" t="str">
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="H68" s="55" t="s">
+      <c r="H68" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="I68" s="66"/>
+      <c r="I68" s="63"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>65</v>
       </c>
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="C69" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="55" t="s">
+      <c r="C69" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="E69" s="55" t="s">
+      <c r="E69" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F69" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G69" s="57" t="str">
-        <f>MID(D69,5,LEN(C69))</f>
+      <c r="F69" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G69" s="54" t="str">
+        <f t="shared" ref="G69:G77" si="2">MID(D69,5,LEN(C69))</f>
         <v>82</v>
       </c>
-      <c r="H69" s="55" t="s">
+      <c r="H69" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="I69" s="66"/>
+      <c r="I69" s="63"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>66</v>
       </c>
-      <c r="B70" s="54" t="s">
+      <c r="B70" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="55" t="s">
+      <c r="C70" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="E70" s="55" t="s">
+      <c r="E70" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F70" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G70" s="57" t="str">
-        <f>MID(D70,5,LEN(C70))</f>
+      <c r="F70" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G70" s="54" t="str">
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
-      <c r="H70" s="55" t="s">
+      <c r="H70" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="I70" s="66"/>
+      <c r="I70" s="63"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>67</v>
       </c>
-      <c r="B71" s="38" t="s">
+      <c r="B71" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="39" t="s">
+      <c r="C71" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E71" s="39" t="s">
+      <c r="E71" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F71" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G71" s="41" t="str">
-        <f>MID(D71,5,LEN(C71))</f>
+      <c r="F71" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="G71" s="38" t="str">
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="H71" s="39" t="s">
+      <c r="H71" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="I71" s="66"/>
+      <c r="I71" s="63"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>68</v>
       </c>
-      <c r="B72" s="38" t="s">
+      <c r="B72" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C72" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="39" t="s">
+      <c r="C72" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E72" s="39" t="s">
+      <c r="E72" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F72" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G72" s="41" t="str">
-        <f>MID(D72,5,LEN(C72))</f>
+      <c r="F72" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="G72" s="38" t="str">
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
-      <c r="H72" s="39" t="s">
+      <c r="H72" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="I72" s="66"/>
+      <c r="I72" s="63"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>69</v>
       </c>
-      <c r="B73" s="30" t="s">
+      <c r="B73" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C73" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="31" t="s">
+      <c r="C73" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E73" s="31" t="s">
+      <c r="E73" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F73" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G73" s="33" t="str">
-        <f>MID(D73,5,LEN(C73))</f>
+      <c r="F73" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G73" s="30" t="str">
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="H73" s="31" t="s">
+      <c r="H73" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="I73" s="66"/>
+      <c r="I73" s="63"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>70</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C74" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="31" t="s">
+      <c r="C74" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E74" s="31" t="s">
+      <c r="E74" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F74" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G74" s="33" t="str">
-        <f>MID(D74,5,LEN(C74))</f>
+      <c r="F74" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G74" s="30" t="str">
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="H74" s="31" t="s">
+      <c r="H74" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="I74" s="66"/>
+      <c r="I74" s="63"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>71</v>
       </c>
-      <c r="B75" s="30" t="s">
+      <c r="B75" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="31" t="s">
+      <c r="C75" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E75" s="31" t="s">
+      <c r="E75" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F75" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G75" s="33" t="str">
-        <f>MID(D75,5,LEN(C75))</f>
+      <c r="F75" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G75" s="30" t="str">
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
-      <c r="H75" s="31" t="s">
+      <c r="H75" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="I75" s="66"/>
+      <c r="I75" s="63"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>72</v>
       </c>
-      <c r="B76" s="30" t="s">
+      <c r="B76" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C76" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="31" t="s">
+      <c r="C76" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E76" s="31" t="s">
+      <c r="E76" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F76" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="G76" s="33" t="str">
-        <f>MID(D76,5,LEN(C76))</f>
+      <c r="F76" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G76" s="30" t="str">
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="H76" s="31" t="s">
+      <c r="H76" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="I76" s="66"/>
+      <c r="I76" s="63"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>73</v>
       </c>
-      <c r="B77" s="62" t="s">
+      <c r="B77" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="C77" s="63" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="63" t="s">
+      <c r="C77" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="E77" s="63" t="s">
+      <c r="E77" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="F77" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="G77" s="45" t="str">
-        <f>MID(D77,5,LEN(C77))</f>
+      <c r="F77" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="G77" s="42" t="str">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="H77" s="65" t="s">
+      <c r="H77" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="I77" s="67"/>
+      <c r="I77" s="64"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
@@ -3861,13 +4083,309 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="79" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="80"/>
+    </row>
+    <row r="2" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="81"/>
+      <c r="E2" s="82"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="70" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="F3" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="70" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="85">
+        <v>1</v>
+      </c>
+      <c r="E4" s="86">
+        <v>2</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="72"/>
+      <c r="H4" s="71"/>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="71"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="85">
+        <f>D4+2</f>
+        <v>3</v>
+      </c>
+      <c r="E5" s="86">
+        <f>E4+2</f>
+        <v>4</v>
+      </c>
+      <c r="F5" s="77" t="s">
+        <v>213</v>
+      </c>
+      <c r="G5" s="73" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="71"/>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="71"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="85">
+        <f t="shared" ref="D6:D13" si="0">D5+2</f>
+        <v>5</v>
+      </c>
+      <c r="E6" s="86">
+        <f t="shared" ref="E6:E13" si="1">E5+2</f>
+        <v>6</v>
+      </c>
+      <c r="F6" s="77" t="s">
+        <v>213</v>
+      </c>
+      <c r="G6" s="73" t="s">
+        <v>223</v>
+      </c>
+      <c r="H6" s="71"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="85">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E7" s="86">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F7" s="78" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="71"/>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="75" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="85">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E8" s="86">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F8" s="78" t="s">
+        <v>215</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="71"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>218</v>
+      </c>
+      <c r="D9" s="85">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E9" s="86">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F9" s="78" t="s">
+        <v>215</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="71"/>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="75" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10" s="85">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E10" s="86">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="F10" s="78" t="s">
+        <v>215</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="71"/>
+    </row>
+    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" s="85">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E11" s="86">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F11" s="78" t="s">
+        <v>215</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="71"/>
+    </row>
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="D12" s="85">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E12" s="86">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F12" s="78" t="s">
+        <v>215</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="71"/>
+    </row>
+    <row r="13" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="75" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" s="87">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E13" s="88">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F13" s="78" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="71"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>